<commit_message>
added state-space simulation data to spreadsheet (for validation comparisons
</commit_message>
<xml_diff>
--- a/documentation/model_validation/state-space/model_parameters.xlsx
+++ b/documentation/model_validation/state-space/model_parameters.xlsx
@@ -1,22 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12354B3B-3C65-4BE2-9A93-3623ED4D9D12}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Single-span" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
   <si>
     <t>Length</t>
   </si>
@@ -79,12 +87,39 @@
   </si>
   <si>
     <t>percent damping</t>
+  </si>
+  <si>
+    <t>damping ratio</t>
+  </si>
+  <si>
+    <t>EI</t>
+  </si>
+  <si>
+    <t>lb-in^2</t>
+  </si>
+  <si>
+    <t>damping coefficient</t>
+  </si>
+  <si>
+    <t>Vehicle Parameters</t>
+  </si>
+  <si>
+    <t>Moment of Inertia (I)</t>
+  </si>
+  <si>
+    <t>Cross sectional area (A)</t>
+  </si>
+  <si>
+    <t>Modulus of Elasticity (E)</t>
+  </si>
+  <si>
+    <t>Material Density</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -114,10 +149,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -127,6 +165,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -175,7 +216,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -208,9 +249,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -243,6 +301,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -418,21 +493,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="E1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -442,8 +527,17 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2">
+        <v>100</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -453,8 +547,17 @@
       <c r="C3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1">
+        <v>63165.5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -464,8 +567,17 @@
       <c r="C4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4">
+        <v>502.65</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -475,8 +587,15 @@
       <c r="C5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="2">
+        <f>F4/(2*SQRT(F2*F3))</f>
+        <v>9.9999014983552181E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -487,7 +606,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -499,60 +618,209 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>100</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B12" s="1">
         <v>63165.5</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>17</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>502.65</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="2">
-        <f>B12/(2*SQRT(B10*B11))</f>
+      <c r="B14" s="2">
+        <f>B13/(2*SQRT(B11*B12))</f>
         <v>9.9999014983552181E-2</v>
       </c>
     </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="E16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>1200</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17">
+        <v>100</v>
+      </c>
+      <c r="G17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="1">
+        <f>B3*B4</f>
+        <v>7500000000000</v>
+      </c>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="1">
+        <v>63165.5</v>
+      </c>
+      <c r="G18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19">
+        <f>B7</f>
+        <v>459999.98087999999</v>
+      </c>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19">
+        <v>502.65</v>
+      </c>
+      <c r="G19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23">
+        <v>1500</v>
+      </c>
+      <c r="C23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24">
+        <v>10</v>
+      </c>
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="1">
+        <v>5000000000</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26">
+        <v>9.9285999999999999E-2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="A22:C22"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -564,7 +832,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>